<commit_message>
ontology, diagram and documentation updated with relative paths and minor fixes
</commit_message>
<xml_diff>
--- a/ontology/requirements/requirements.xlsx
+++ b/ontology/requirements/requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/rml/rml-io/ontology/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/forks/rml-io/ontology/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F129F14-C1C1-964E-A1C4-FE96660D8549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1239C50-F91B-AF46-9619-ADC9EA5F22D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Identifier</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>rml-io-r6</t>
+  </si>
+  <si>
+    <t>rml-io-r7</t>
+  </si>
+  <si>
+    <t>Logical sources and logical targets may indicate relative paths to resources</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,8 +559,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>

</xml_diff>